<commit_message>
Timetable and Journal updated
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="48">
   <si>
     <t>Tätigkeit</t>
   </si>
@@ -150,13 +150,25 @@
   </si>
   <si>
     <t>complete documentation</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>Milestone 1</t>
+  </si>
+  <si>
+    <t>Milestone 2</t>
+  </si>
+  <si>
+    <t>Milestone 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +183,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -203,11 +221,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -242,11 +306,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="68">
     <dxf>
       <font>
         <color rgb="FF0070C0"/>
@@ -279,6 +355,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF66FF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
       </font>
       <fill>
@@ -289,6 +395,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF66FF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF00B050"/>
       </font>
       <fill>
@@ -299,6 +425,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF0070C0"/>
       </font>
       <fill>
@@ -309,6 +445,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
       </font>
       <fill>
@@ -319,6 +465,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF00B050"/>
       </font>
       <fill>
@@ -329,16 +485,531 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF66FF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF0070C0"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF66FF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF66FF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF66FF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF66FF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF66FF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF66"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -627,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="G27:R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -640,7 +1311,7 @@
     <col min="3" max="78" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="57.75" customHeight="1">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="57.75" customHeight="1">
       <c r="A1" s="3"/>
       <c r="C1" s="8" t="s">
         <v>29</v>
@@ -685,7 +1356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -696,18 +1367,19 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="15"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="P2" s="14"/>
+      <c r="Q2" s="17"/>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
@@ -720,18 +1392,19 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="P3" s="14"/>
+      <c r="Q3" s="17"/>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="13"/>
       <c r="B4" s="7" t="s">
         <v>16</v>
@@ -742,18 +1415,19 @@
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="15"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="P4" s="14"/>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
@@ -766,18 +1440,19 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="P5" s="14"/>
+      <c r="Q5" s="17"/>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="13"/>
       <c r="B6" s="7" t="s">
         <v>16</v>
@@ -790,18 +1465,19 @@
         <v>3</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="P6" s="14"/>
+      <c r="Q6" s="17"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="13" t="s">
         <v>18</v>
       </c>
@@ -816,22 +1492,23 @@
       <c r="F7" s="5">
         <v>1</v>
       </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="G7" s="14">
+        <v>1</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="P7" s="14"/>
+      <c r="Q7" s="17"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="13"/>
       <c r="B8" s="7" t="s">
         <v>16</v>
@@ -842,18 +1519,19 @@
         <v>2</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="15"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="P8" s="14"/>
+      <c r="Q8" s="17"/>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="13" t="s">
         <v>19</v>
       </c>
@@ -868,20 +1546,21 @@
       <c r="F9" s="5">
         <v>1</v>
       </c>
-      <c r="G9" s="5">
-        <v>1</v>
-      </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="G9" s="14">
+        <v>1</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="P9" s="14"/>
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="13"/>
       <c r="B10" s="7" t="s">
         <v>16</v>
@@ -892,18 +1571,19 @@
         <v>2</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="P10" s="14"/>
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="12" t="s">
         <v>23</v>
       </c>
@@ -914,22 +1594,23 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5"/>
+      <c r="G11" s="14">
+        <v>1</v>
+      </c>
+      <c r="H11" s="14">
+        <v>1</v>
+      </c>
+      <c r="I11" s="15"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="P11" s="14"/>
+      <c r="Q11" s="17"/>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="13"/>
       <c r="B12" s="7" t="s">
         <v>16</v>
@@ -937,19 +1618,24 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="F12" s="5">
+        <v>4</v>
+      </c>
+      <c r="G12" s="14">
+        <v>2</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="P12" s="14"/>
+      <c r="Q12" s="17"/>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="12" t="s">
         <v>20</v>
       </c>
@@ -960,22 +1646,23 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5">
+      <c r="G13" s="14"/>
+      <c r="H13" s="14">
+        <v>1</v>
+      </c>
+      <c r="I13" s="15">
         <v>1</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="P13" s="14"/>
+      <c r="Q13" s="17"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="13"/>
       <c r="B14" s="7" t="s">
         <v>16</v>
@@ -984,18 +1671,21 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="G14" s="14">
+        <v>4</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="P14" s="14"/>
+      <c r="Q14" s="17"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
@@ -1006,9 +1696,9 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5">
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15">
         <v>1</v>
       </c>
       <c r="J15" s="5">
@@ -1017,15 +1707,16 @@
       <c r="K15" s="5">
         <v>1</v>
       </c>
-      <c r="L15" s="5">
-        <v>1</v>
-      </c>
-      <c r="M15" s="5"/>
+      <c r="L15" s="14">
+        <v>1</v>
+      </c>
+      <c r="M15" s="15"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="P15" s="14"/>
+      <c r="Q15" s="17"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="13"/>
       <c r="B16" s="7" t="s">
         <v>16</v>
@@ -1034,18 +1725,21 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="G16" s="14">
+        <v>4</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="15"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="P16" s="14"/>
+      <c r="Q16" s="17"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
@@ -1056,24 +1750,25 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="5">
         <v>1</v>
       </c>
       <c r="K17" s="5">
         <v>1</v>
       </c>
-      <c r="L17" s="5">
-        <v>1</v>
-      </c>
-      <c r="M17" s="5"/>
+      <c r="L17" s="14">
+        <v>1</v>
+      </c>
+      <c r="M17" s="15"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="P17" s="14"/>
+      <c r="Q17" s="17"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="13"/>
       <c r="B18" s="7" t="s">
         <v>16</v>
@@ -1082,18 +1777,19 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="15"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="P18" s="14"/>
+      <c r="Q18" s="17"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="12" t="s">
         <v>25</v>
       </c>
@@ -1104,24 +1800,25 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="5">
         <v>1</v>
       </c>
       <c r="K19" s="5">
         <v>1</v>
       </c>
-      <c r="L19" s="5">
-        <v>1</v>
-      </c>
-      <c r="M19" s="5"/>
+      <c r="L19" s="14">
+        <v>1</v>
+      </c>
+      <c r="M19" s="15"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="P19" s="14"/>
+      <c r="Q19" s="17"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="13"/>
       <c r="B20" s="7" t="s">
         <v>16</v>
@@ -1130,18 +1827,19 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="P20" s="14"/>
+      <c r="Q20" s="17"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
@@ -1152,13 +1850,13 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="5">
-        <v>1</v>
-      </c>
-      <c r="H21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="5">
+      <c r="G21" s="14">
+        <v>1</v>
+      </c>
+      <c r="H21" s="14">
+        <v>1</v>
+      </c>
+      <c r="I21" s="15">
         <v>1</v>
       </c>
       <c r="J21" s="5">
@@ -1167,15 +1865,16 @@
       <c r="K21" s="5">
         <v>1</v>
       </c>
-      <c r="L21" s="5">
-        <v>1</v>
-      </c>
-      <c r="M21" s="5"/>
+      <c r="L21" s="14">
+        <v>1</v>
+      </c>
+      <c r="M21" s="15"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="P21" s="14"/>
+      <c r="Q21" s="17"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="13"/>
       <c r="B22" s="7" t="s">
         <v>16</v>
@@ -1184,18 +1883,21 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="G22" s="14">
+        <v>2</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="15"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="P22" s="14"/>
+      <c r="Q22" s="17"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
@@ -1206,13 +1908,13 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5">
+      <c r="L23" s="14"/>
+      <c r="M23" s="15">
         <v>1</v>
       </c>
       <c r="N23" s="5">
@@ -1221,11 +1923,12 @@
       <c r="O23" s="5">
         <v>1</v>
       </c>
-      <c r="P23" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="P23" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="17"/>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="13"/>
       <c r="B24" s="7" t="s">
         <v>16</v>
@@ -1234,18 +1937,19 @@
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="15"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="P24" s="14"/>
+      <c r="Q24" s="17"/>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="13" t="s">
         <v>27</v>
       </c>
@@ -1256,13 +1960,13 @@
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5">
+      <c r="L25" s="14"/>
+      <c r="M25" s="15">
         <v>1</v>
       </c>
       <c r="N25" s="5">
@@ -1271,11 +1975,12 @@
       <c r="O25" s="5">
         <v>1</v>
       </c>
-      <c r="P25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="P25" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="17"/>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="13"/>
       <c r="B26" s="7" t="s">
         <v>16</v>
@@ -1284,38 +1989,69 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="15"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="P26" s="14"/>
+      <c r="Q26" s="17"/>
+    </row>
+    <row r="27" spans="1:18" ht="15" customHeight="1">
       <c r="A27" s="11"/>
       <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="H27" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" s="16"/>
+      <c r="L27" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M27" s="16"/>
+      <c r="P27" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q27" s="19"/>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="11"/>
       <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="G28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="11"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:18">
       <c r="A30" s="11"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:18">
       <c r="A31" s="11"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:18">
       <c r="A32" s="11"/>
       <c r="B32" s="2"/>
     </row>
@@ -1328,7 +2064,13 @@
       <c r="B34" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="22">
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="O28:R28"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
@@ -1347,14 +2089,28 @@
     <mergeCell ref="A13:A14"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:P26 Q21">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:P26">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
-      <formula>3</formula>
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1364,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27:R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1377,7 +2133,7 @@
     <col min="3" max="78" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="57.75" customHeight="1">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="57.75" customHeight="1">
       <c r="A1" s="3"/>
       <c r="C1" s="8" t="s">
         <v>29</v>
@@ -1422,7 +2178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
@@ -1445,15 +2201,15 @@
         <f>IF(Deutsch!F2="","",Deutsch!F2)</f>
         <v/>
       </c>
-      <c r="G2" s="5" t="str">
+      <c r="G2" s="14" t="str">
         <f>IF(Deutsch!G2="","",Deutsch!G2)</f>
         <v/>
       </c>
-      <c r="H2" s="5" t="str">
+      <c r="H2" s="14" t="str">
         <f>IF(Deutsch!H2="","",Deutsch!H2)</f>
         <v/>
       </c>
-      <c r="I2" s="5" t="str">
+      <c r="I2" s="15" t="str">
         <f>IF(Deutsch!I2="","",Deutsch!I2)</f>
         <v/>
       </c>
@@ -1465,11 +2221,11 @@
         <f>IF(Deutsch!K2="","",Deutsch!K2)</f>
         <v/>
       </c>
-      <c r="L2" s="5" t="str">
+      <c r="L2" s="14" t="str">
         <f>IF(Deutsch!L2="","",Deutsch!L2)</f>
         <v/>
       </c>
-      <c r="M2" s="5" t="str">
+      <c r="M2" s="15" t="str">
         <f>IF(Deutsch!M2="","",Deutsch!M2)</f>
         <v/>
       </c>
@@ -1481,12 +2237,13 @@
         <f>IF(Deutsch!O2="","",Deutsch!O2)</f>
         <v/>
       </c>
-      <c r="P2" s="5" t="str">
+      <c r="P2" s="14" t="str">
         <f>IF(Deutsch!P2="","",Deutsch!P2)</f>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="17"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>32</v>
       </c>
@@ -1509,15 +2266,15 @@
         <f>IF(Deutsch!F3="","",Deutsch!F3)</f>
         <v/>
       </c>
-      <c r="G3" s="5" t="str">
+      <c r="G3" s="14" t="str">
         <f>IF(Deutsch!G3="","",Deutsch!G3)</f>
         <v/>
       </c>
-      <c r="H3" s="5" t="str">
+      <c r="H3" s="14" t="str">
         <f>IF(Deutsch!H3="","",Deutsch!H3)</f>
         <v/>
       </c>
-      <c r="I3" s="5" t="str">
+      <c r="I3" s="15" t="str">
         <f>IF(Deutsch!I3="","",Deutsch!I3)</f>
         <v/>
       </c>
@@ -1529,11 +2286,11 @@
         <f>IF(Deutsch!K3="","",Deutsch!K3)</f>
         <v/>
       </c>
-      <c r="L3" s="5" t="str">
+      <c r="L3" s="14" t="str">
         <f>IF(Deutsch!L3="","",Deutsch!L3)</f>
         <v/>
       </c>
-      <c r="M3" s="5" t="str">
+      <c r="M3" s="15" t="str">
         <f>IF(Deutsch!M3="","",Deutsch!M3)</f>
         <v/>
       </c>
@@ -1545,12 +2302,13 @@
         <f>IF(Deutsch!O3="","",Deutsch!O3)</f>
         <v/>
       </c>
-      <c r="P3" s="5" t="str">
+      <c r="P3" s="14" t="str">
         <f>IF(Deutsch!P3="","",Deutsch!P3)</f>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" s="17"/>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="13"/>
       <c r="B4" s="7" t="s">
         <v>16</v>
@@ -1571,15 +2329,15 @@
         <f>IF(Deutsch!F4="","",Deutsch!F4)</f>
         <v/>
       </c>
-      <c r="G4" s="5" t="str">
+      <c r="G4" s="14" t="str">
         <f>IF(Deutsch!G4="","",Deutsch!G4)</f>
         <v/>
       </c>
-      <c r="H4" s="5" t="str">
+      <c r="H4" s="14" t="str">
         <f>IF(Deutsch!H4="","",Deutsch!H4)</f>
         <v/>
       </c>
-      <c r="I4" s="5" t="str">
+      <c r="I4" s="15" t="str">
         <f>IF(Deutsch!I4="","",Deutsch!I4)</f>
         <v/>
       </c>
@@ -1591,11 +2349,11 @@
         <f>IF(Deutsch!K4="","",Deutsch!K4)</f>
         <v/>
       </c>
-      <c r="L4" s="5" t="str">
+      <c r="L4" s="14" t="str">
         <f>IF(Deutsch!L4="","",Deutsch!L4)</f>
         <v/>
       </c>
-      <c r="M4" s="5" t="str">
+      <c r="M4" s="15" t="str">
         <f>IF(Deutsch!M4="","",Deutsch!M4)</f>
         <v/>
       </c>
@@ -1607,12 +2365,13 @@
         <f>IF(Deutsch!O4="","",Deutsch!O4)</f>
         <v/>
       </c>
-      <c r="P4" s="5" t="str">
+      <c r="P4" s="14" t="str">
         <f>IF(Deutsch!P4="","",Deutsch!P4)</f>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="13" t="s">
         <v>33</v>
       </c>
@@ -1635,15 +2394,15 @@
         <f>IF(Deutsch!F5="","",Deutsch!F5)</f>
         <v/>
       </c>
-      <c r="G5" s="5" t="str">
+      <c r="G5" s="14" t="str">
         <f>IF(Deutsch!G5="","",Deutsch!G5)</f>
         <v/>
       </c>
-      <c r="H5" s="5" t="str">
+      <c r="H5" s="14" t="str">
         <f>IF(Deutsch!H5="","",Deutsch!H5)</f>
         <v/>
       </c>
-      <c r="I5" s="5" t="str">
+      <c r="I5" s="15" t="str">
         <f>IF(Deutsch!I5="","",Deutsch!I5)</f>
         <v/>
       </c>
@@ -1655,11 +2414,11 @@
         <f>IF(Deutsch!K5="","",Deutsch!K5)</f>
         <v/>
       </c>
-      <c r="L5" s="5" t="str">
+      <c r="L5" s="14" t="str">
         <f>IF(Deutsch!L5="","",Deutsch!L5)</f>
         <v/>
       </c>
-      <c r="M5" s="5" t="str">
+      <c r="M5" s="15" t="str">
         <f>IF(Deutsch!M5="","",Deutsch!M5)</f>
         <v/>
       </c>
@@ -1671,12 +2430,13 @@
         <f>IF(Deutsch!O5="","",Deutsch!O5)</f>
         <v/>
       </c>
-      <c r="P5" s="5" t="str">
+      <c r="P5" s="14" t="str">
         <f>IF(Deutsch!P5="","",Deutsch!P5)</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" s="17"/>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="13"/>
       <c r="B6" s="7" t="s">
         <v>16</v>
@@ -1697,15 +2457,15 @@
         <f>IF(Deutsch!F6="","",Deutsch!F6)</f>
         <v/>
       </c>
-      <c r="G6" s="5" t="str">
+      <c r="G6" s="14" t="str">
         <f>IF(Deutsch!G6="","",Deutsch!G6)</f>
         <v/>
       </c>
-      <c r="H6" s="5" t="str">
+      <c r="H6" s="14" t="str">
         <f>IF(Deutsch!H6="","",Deutsch!H6)</f>
         <v/>
       </c>
-      <c r="I6" s="5" t="str">
+      <c r="I6" s="15" t="str">
         <f>IF(Deutsch!I6="","",Deutsch!I6)</f>
         <v/>
       </c>
@@ -1717,11 +2477,11 @@
         <f>IF(Deutsch!K6="","",Deutsch!K6)</f>
         <v/>
       </c>
-      <c r="L6" s="5" t="str">
+      <c r="L6" s="14" t="str">
         <f>IF(Deutsch!L6="","",Deutsch!L6)</f>
         <v/>
       </c>
-      <c r="M6" s="5" t="str">
+      <c r="M6" s="15" t="str">
         <f>IF(Deutsch!M6="","",Deutsch!M6)</f>
         <v/>
       </c>
@@ -1733,12 +2493,13 @@
         <f>IF(Deutsch!O6="","",Deutsch!O6)</f>
         <v/>
       </c>
-      <c r="P6" s="5" t="str">
+      <c r="P6" s="14" t="str">
         <f>IF(Deutsch!P6="","",Deutsch!P6)</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" s="17"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="13" t="s">
         <v>34</v>
       </c>
@@ -1761,15 +2522,15 @@
         <f>IF(Deutsch!F7="","",Deutsch!F7)</f>
         <v>1</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="14">
         <f>IF(Deutsch!G7="","",Deutsch!G7)</f>
         <v>1</v>
       </c>
-      <c r="H7" s="5" t="str">
+      <c r="H7" s="14" t="str">
         <f>IF(Deutsch!H7="","",Deutsch!H7)</f>
         <v/>
       </c>
-      <c r="I7" s="5" t="str">
+      <c r="I7" s="15" t="str">
         <f>IF(Deutsch!I7="","",Deutsch!I7)</f>
         <v/>
       </c>
@@ -1781,11 +2542,11 @@
         <f>IF(Deutsch!K7="","",Deutsch!K7)</f>
         <v/>
       </c>
-      <c r="L7" s="5" t="str">
+      <c r="L7" s="14" t="str">
         <f>IF(Deutsch!L7="","",Deutsch!L7)</f>
         <v/>
       </c>
-      <c r="M7" s="5" t="str">
+      <c r="M7" s="15" t="str">
         <f>IF(Deutsch!M7="","",Deutsch!M7)</f>
         <v/>
       </c>
@@ -1797,12 +2558,13 @@
         <f>IF(Deutsch!O7="","",Deutsch!O7)</f>
         <v/>
       </c>
-      <c r="P7" s="5" t="str">
+      <c r="P7" s="14" t="str">
         <f>IF(Deutsch!P7="","",Deutsch!P7)</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" s="17"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="13"/>
       <c r="B8" s="7" t="s">
         <v>16</v>
@@ -1823,15 +2585,15 @@
         <f>IF(Deutsch!F8="","",Deutsch!F8)</f>
         <v/>
       </c>
-      <c r="G8" s="5" t="str">
+      <c r="G8" s="14" t="str">
         <f>IF(Deutsch!G8="","",Deutsch!G8)</f>
         <v/>
       </c>
-      <c r="H8" s="5" t="str">
+      <c r="H8" s="14" t="str">
         <f>IF(Deutsch!H8="","",Deutsch!H8)</f>
         <v/>
       </c>
-      <c r="I8" s="5" t="str">
+      <c r="I8" s="15" t="str">
         <f>IF(Deutsch!I8="","",Deutsch!I8)</f>
         <v/>
       </c>
@@ -1843,11 +2605,11 @@
         <f>IF(Deutsch!K8="","",Deutsch!K8)</f>
         <v/>
       </c>
-      <c r="L8" s="5" t="str">
+      <c r="L8" s="14" t="str">
         <f>IF(Deutsch!L8="","",Deutsch!L8)</f>
         <v/>
       </c>
-      <c r="M8" s="5" t="str">
+      <c r="M8" s="15" t="str">
         <f>IF(Deutsch!M8="","",Deutsch!M8)</f>
         <v/>
       </c>
@@ -1859,12 +2621,13 @@
         <f>IF(Deutsch!O8="","",Deutsch!O8)</f>
         <v/>
       </c>
-      <c r="P8" s="5" t="str">
+      <c r="P8" s="14" t="str">
         <f>IF(Deutsch!P8="","",Deutsch!P8)</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8" s="17"/>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="13" t="s">
         <v>35</v>
       </c>
@@ -1887,15 +2650,15 @@
         <f>IF(Deutsch!F9="","",Deutsch!F9)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="14">
         <f>IF(Deutsch!G9="","",Deutsch!G9)</f>
         <v>1</v>
       </c>
-      <c r="H9" s="5" t="str">
+      <c r="H9" s="14" t="str">
         <f>IF(Deutsch!H9="","",Deutsch!H9)</f>
         <v/>
       </c>
-      <c r="I9" s="5" t="str">
+      <c r="I9" s="15" t="str">
         <f>IF(Deutsch!I9="","",Deutsch!I9)</f>
         <v/>
       </c>
@@ -1907,11 +2670,11 @@
         <f>IF(Deutsch!K9="","",Deutsch!K9)</f>
         <v/>
       </c>
-      <c r="L9" s="5" t="str">
+      <c r="L9" s="14" t="str">
         <f>IF(Deutsch!L9="","",Deutsch!L9)</f>
         <v/>
       </c>
-      <c r="M9" s="5" t="str">
+      <c r="M9" s="15" t="str">
         <f>IF(Deutsch!M9="","",Deutsch!M9)</f>
         <v/>
       </c>
@@ -1923,12 +2686,13 @@
         <f>IF(Deutsch!O9="","",Deutsch!O9)</f>
         <v/>
       </c>
-      <c r="P9" s="5" t="str">
+      <c r="P9" s="14" t="str">
         <f>IF(Deutsch!P9="","",Deutsch!P9)</f>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="13"/>
       <c r="B10" s="7" t="s">
         <v>16</v>
@@ -1949,15 +2713,15 @@
         <f>IF(Deutsch!F10="","",Deutsch!F10)</f>
         <v/>
       </c>
-      <c r="G10" s="5" t="str">
+      <c r="G10" s="14" t="str">
         <f>IF(Deutsch!G10="","",Deutsch!G10)</f>
         <v/>
       </c>
-      <c r="H10" s="5" t="str">
+      <c r="H10" s="14" t="str">
         <f>IF(Deutsch!H10="","",Deutsch!H10)</f>
         <v/>
       </c>
-      <c r="I10" s="5" t="str">
+      <c r="I10" s="15" t="str">
         <f>IF(Deutsch!I10="","",Deutsch!I10)</f>
         <v/>
       </c>
@@ -1969,11 +2733,11 @@
         <f>IF(Deutsch!K10="","",Deutsch!K10)</f>
         <v/>
       </c>
-      <c r="L10" s="5" t="str">
+      <c r="L10" s="14" t="str">
         <f>IF(Deutsch!L10="","",Deutsch!L10)</f>
         <v/>
       </c>
-      <c r="M10" s="5" t="str">
+      <c r="M10" s="15" t="str">
         <f>IF(Deutsch!M10="","",Deutsch!M10)</f>
         <v/>
       </c>
@@ -1985,12 +2749,13 @@
         <f>IF(Deutsch!O10="","",Deutsch!O10)</f>
         <v/>
       </c>
-      <c r="P10" s="5" t="str">
+      <c r="P10" s="14" t="str">
         <f>IF(Deutsch!P10="","",Deutsch!P10)</f>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
@@ -2013,15 +2778,15 @@
         <f>IF(Deutsch!F11="","",Deutsch!F11)</f>
         <v/>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="14">
         <f>IF(Deutsch!G11="","",Deutsch!G11)</f>
         <v>1</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="14">
         <f>IF(Deutsch!H11="","",Deutsch!H11)</f>
         <v>1</v>
       </c>
-      <c r="I11" s="5" t="str">
+      <c r="I11" s="15" t="str">
         <f>IF(Deutsch!I11="","",Deutsch!I11)</f>
         <v/>
       </c>
@@ -2033,11 +2798,11 @@
         <f>IF(Deutsch!K11="","",Deutsch!K11)</f>
         <v/>
       </c>
-      <c r="L11" s="5" t="str">
+      <c r="L11" s="14" t="str">
         <f>IF(Deutsch!L11="","",Deutsch!L11)</f>
         <v/>
       </c>
-      <c r="M11" s="5" t="str">
+      <c r="M11" s="15" t="str">
         <f>IF(Deutsch!M11="","",Deutsch!M11)</f>
         <v/>
       </c>
@@ -2049,12 +2814,13 @@
         <f>IF(Deutsch!O11="","",Deutsch!O11)</f>
         <v/>
       </c>
-      <c r="P11" s="5" t="str">
+      <c r="P11" s="14" t="str">
         <f>IF(Deutsch!P11="","",Deutsch!P11)</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="17"/>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="13"/>
       <c r="B12" s="7" t="s">
         <v>16</v>
@@ -2071,19 +2837,19 @@
         <f>IF(Deutsch!E12="","",Deutsch!E12)</f>
         <v/>
       </c>
-      <c r="F12" s="5" t="str">
+      <c r="F12" s="5">
         <f>IF(Deutsch!F12="","",Deutsch!F12)</f>
-        <v/>
-      </c>
-      <c r="G12" s="5" t="str">
+        <v>4</v>
+      </c>
+      <c r="G12" s="14">
         <f>IF(Deutsch!G12="","",Deutsch!G12)</f>
-        <v/>
-      </c>
-      <c r="H12" s="5" t="str">
+        <v>2</v>
+      </c>
+      <c r="H12" s="14" t="str">
         <f>IF(Deutsch!H12="","",Deutsch!H12)</f>
         <v/>
       </c>
-      <c r="I12" s="5" t="str">
+      <c r="I12" s="15" t="str">
         <f>IF(Deutsch!I12="","",Deutsch!I12)</f>
         <v/>
       </c>
@@ -2095,11 +2861,11 @@
         <f>IF(Deutsch!K12="","",Deutsch!K12)</f>
         <v/>
       </c>
-      <c r="L12" s="5" t="str">
+      <c r="L12" s="14" t="str">
         <f>IF(Deutsch!L12="","",Deutsch!L12)</f>
         <v/>
       </c>
-      <c r="M12" s="5" t="str">
+      <c r="M12" s="15" t="str">
         <f>IF(Deutsch!M12="","",Deutsch!M12)</f>
         <v/>
       </c>
@@ -2111,12 +2877,13 @@
         <f>IF(Deutsch!O12="","",Deutsch!O12)</f>
         <v/>
       </c>
-      <c r="P12" s="5" t="str">
+      <c r="P12" s="14" t="str">
         <f>IF(Deutsch!P12="","",Deutsch!P12)</f>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" s="17"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1">
       <c r="A13" s="12" t="s">
         <v>37</v>
       </c>
@@ -2139,15 +2906,15 @@
         <f>IF(Deutsch!F13="","",Deutsch!F13)</f>
         <v/>
       </c>
-      <c r="G13" s="5" t="str">
+      <c r="G13" s="14" t="str">
         <f>IF(Deutsch!G13="","",Deutsch!G13)</f>
         <v/>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="14">
         <f>IF(Deutsch!H13="","",Deutsch!H13)</f>
         <v>1</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="15">
         <f>IF(Deutsch!I13="","",Deutsch!I13)</f>
         <v>1</v>
       </c>
@@ -2159,11 +2926,11 @@
         <f>IF(Deutsch!K13="","",Deutsch!K13)</f>
         <v/>
       </c>
-      <c r="L13" s="5" t="str">
+      <c r="L13" s="14" t="str">
         <f>IF(Deutsch!L13="","",Deutsch!L13)</f>
         <v/>
       </c>
-      <c r="M13" s="5" t="str">
+      <c r="M13" s="15" t="str">
         <f>IF(Deutsch!M13="","",Deutsch!M13)</f>
         <v/>
       </c>
@@ -2175,12 +2942,13 @@
         <f>IF(Deutsch!O13="","",Deutsch!O13)</f>
         <v/>
       </c>
-      <c r="P13" s="5" t="str">
+      <c r="P13" s="14" t="str">
         <f>IF(Deutsch!P13="","",Deutsch!P13)</f>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" s="17"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="13"/>
       <c r="B14" s="7" t="s">
         <v>16</v>
@@ -2201,15 +2969,15 @@
         <f>IF(Deutsch!F14="","",Deutsch!F14)</f>
         <v/>
       </c>
-      <c r="G14" s="5" t="str">
+      <c r="G14" s="14">
         <f>IF(Deutsch!G14="","",Deutsch!G14)</f>
-        <v/>
-      </c>
-      <c r="H14" s="5" t="str">
+        <v>4</v>
+      </c>
+      <c r="H14" s="14" t="str">
         <f>IF(Deutsch!H14="","",Deutsch!H14)</f>
         <v/>
       </c>
-      <c r="I14" s="5" t="str">
+      <c r="I14" s="15" t="str">
         <f>IF(Deutsch!I14="","",Deutsch!I14)</f>
         <v/>
       </c>
@@ -2221,11 +2989,11 @@
         <f>IF(Deutsch!K14="","",Deutsch!K14)</f>
         <v/>
       </c>
-      <c r="L14" s="5" t="str">
+      <c r="L14" s="14" t="str">
         <f>IF(Deutsch!L14="","",Deutsch!L14)</f>
         <v/>
       </c>
-      <c r="M14" s="5" t="str">
+      <c r="M14" s="15" t="str">
         <f>IF(Deutsch!M14="","",Deutsch!M14)</f>
         <v/>
       </c>
@@ -2237,12 +3005,13 @@
         <f>IF(Deutsch!O14="","",Deutsch!O14)</f>
         <v/>
       </c>
-      <c r="P14" s="5" t="str">
+      <c r="P14" s="14" t="str">
         <f>IF(Deutsch!P14="","",Deutsch!P14)</f>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14" s="17"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>38</v>
       </c>
@@ -2265,15 +3034,15 @@
         <f>IF(Deutsch!F15="","",Deutsch!F15)</f>
         <v/>
       </c>
-      <c r="G15" s="5" t="str">
+      <c r="G15" s="14" t="str">
         <f>IF(Deutsch!G15="","",Deutsch!G15)</f>
         <v/>
       </c>
-      <c r="H15" s="5" t="str">
+      <c r="H15" s="14" t="str">
         <f>IF(Deutsch!H15="","",Deutsch!H15)</f>
         <v/>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="15">
         <f>IF(Deutsch!I15="","",Deutsch!I15)</f>
         <v>1</v>
       </c>
@@ -2285,11 +3054,11 @@
         <f>IF(Deutsch!K15="","",Deutsch!K15)</f>
         <v>1</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="14">
         <f>IF(Deutsch!L15="","",Deutsch!L15)</f>
         <v>1</v>
       </c>
-      <c r="M15" s="5" t="str">
+      <c r="M15" s="15" t="str">
         <f>IF(Deutsch!M15="","",Deutsch!M15)</f>
         <v/>
       </c>
@@ -2301,12 +3070,13 @@
         <f>IF(Deutsch!O15="","",Deutsch!O15)</f>
         <v/>
       </c>
-      <c r="P15" s="5" t="str">
+      <c r="P15" s="14" t="str">
         <f>IF(Deutsch!P15="","",Deutsch!P15)</f>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" s="17"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="13"/>
       <c r="B16" s="7" t="s">
         <v>16</v>
@@ -2327,15 +3097,15 @@
         <f>IF(Deutsch!F16="","",Deutsch!F16)</f>
         <v/>
       </c>
-      <c r="G16" s="5" t="str">
+      <c r="G16" s="14">
         <f>IF(Deutsch!G16="","",Deutsch!G16)</f>
-        <v/>
-      </c>
-      <c r="H16" s="5" t="str">
+        <v>4</v>
+      </c>
+      <c r="H16" s="14" t="str">
         <f>IF(Deutsch!H16="","",Deutsch!H16)</f>
         <v/>
       </c>
-      <c r="I16" s="5" t="str">
+      <c r="I16" s="15" t="str">
         <f>IF(Deutsch!I16="","",Deutsch!I16)</f>
         <v/>
       </c>
@@ -2347,11 +3117,11 @@
         <f>IF(Deutsch!K16="","",Deutsch!K16)</f>
         <v/>
       </c>
-      <c r="L16" s="5" t="str">
+      <c r="L16" s="14" t="str">
         <f>IF(Deutsch!L16="","",Deutsch!L16)</f>
         <v/>
       </c>
-      <c r="M16" s="5" t="str">
+      <c r="M16" s="15" t="str">
         <f>IF(Deutsch!M16="","",Deutsch!M16)</f>
         <v/>
       </c>
@@ -2363,12 +3133,13 @@
         <f>IF(Deutsch!O16="","",Deutsch!O16)</f>
         <v/>
       </c>
-      <c r="P16" s="5" t="str">
+      <c r="P16" s="14" t="str">
         <f>IF(Deutsch!P16="","",Deutsch!P16)</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" s="17"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="12" t="s">
         <v>39</v>
       </c>
@@ -2391,15 +3162,15 @@
         <f>IF(Deutsch!F17="","",Deutsch!F17)</f>
         <v/>
       </c>
-      <c r="G17" s="5" t="str">
+      <c r="G17" s="14" t="str">
         <f>IF(Deutsch!G17="","",Deutsch!G17)</f>
         <v/>
       </c>
-      <c r="H17" s="5" t="str">
+      <c r="H17" s="14" t="str">
         <f>IF(Deutsch!H17="","",Deutsch!H17)</f>
         <v/>
       </c>
-      <c r="I17" s="5" t="str">
+      <c r="I17" s="15" t="str">
         <f>IF(Deutsch!I17="","",Deutsch!I17)</f>
         <v/>
       </c>
@@ -2411,11 +3182,11 @@
         <f>IF(Deutsch!K17="","",Deutsch!K17)</f>
         <v>1</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="14">
         <f>IF(Deutsch!L17="","",Deutsch!L17)</f>
         <v>1</v>
       </c>
-      <c r="M17" s="5" t="str">
+      <c r="M17" s="15" t="str">
         <f>IF(Deutsch!M17="","",Deutsch!M17)</f>
         <v/>
       </c>
@@ -2427,12 +3198,13 @@
         <f>IF(Deutsch!O17="","",Deutsch!O17)</f>
         <v/>
       </c>
-      <c r="P17" s="5" t="str">
+      <c r="P17" s="14" t="str">
         <f>IF(Deutsch!P17="","",Deutsch!P17)</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" s="17"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="13"/>
       <c r="B18" s="7" t="s">
         <v>16</v>
@@ -2453,15 +3225,15 @@
         <f>IF(Deutsch!F18="","",Deutsch!F18)</f>
         <v/>
       </c>
-      <c r="G18" s="5" t="str">
+      <c r="G18" s="14" t="str">
         <f>IF(Deutsch!G18="","",Deutsch!G18)</f>
         <v/>
       </c>
-      <c r="H18" s="5" t="str">
+      <c r="H18" s="14" t="str">
         <f>IF(Deutsch!H18="","",Deutsch!H18)</f>
         <v/>
       </c>
-      <c r="I18" s="5" t="str">
+      <c r="I18" s="15" t="str">
         <f>IF(Deutsch!I18="","",Deutsch!I18)</f>
         <v/>
       </c>
@@ -2473,11 +3245,11 @@
         <f>IF(Deutsch!K18="","",Deutsch!K18)</f>
         <v/>
       </c>
-      <c r="L18" s="5" t="str">
+      <c r="L18" s="14" t="str">
         <f>IF(Deutsch!L18="","",Deutsch!L18)</f>
         <v/>
       </c>
-      <c r="M18" s="5" t="str">
+      <c r="M18" s="15" t="str">
         <f>IF(Deutsch!M18="","",Deutsch!M18)</f>
         <v/>
       </c>
@@ -2489,12 +3261,13 @@
         <f>IF(Deutsch!O18="","",Deutsch!O18)</f>
         <v/>
       </c>
-      <c r="P18" s="5" t="str">
+      <c r="P18" s="14" t="str">
         <f>IF(Deutsch!P18="","",Deutsch!P18)</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" s="17"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="12" t="s">
         <v>40</v>
       </c>
@@ -2517,15 +3290,15 @@
         <f>IF(Deutsch!F19="","",Deutsch!F19)</f>
         <v/>
       </c>
-      <c r="G19" s="5" t="str">
+      <c r="G19" s="14" t="str">
         <f>IF(Deutsch!G19="","",Deutsch!G19)</f>
         <v/>
       </c>
-      <c r="H19" s="5" t="str">
+      <c r="H19" s="14" t="str">
         <f>IF(Deutsch!H19="","",Deutsch!H19)</f>
         <v/>
       </c>
-      <c r="I19" s="5" t="str">
+      <c r="I19" s="15" t="str">
         <f>IF(Deutsch!I19="","",Deutsch!I19)</f>
         <v/>
       </c>
@@ -2537,11 +3310,11 @@
         <f>IF(Deutsch!K19="","",Deutsch!K19)</f>
         <v>1</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="14">
         <f>IF(Deutsch!L19="","",Deutsch!L19)</f>
         <v>1</v>
       </c>
-      <c r="M19" s="5" t="str">
+      <c r="M19" s="15" t="str">
         <f>IF(Deutsch!M19="","",Deutsch!M19)</f>
         <v/>
       </c>
@@ -2553,12 +3326,13 @@
         <f>IF(Deutsch!O19="","",Deutsch!O19)</f>
         <v/>
       </c>
-      <c r="P19" s="5" t="str">
+      <c r="P19" s="14" t="str">
         <f>IF(Deutsch!P19="","",Deutsch!P19)</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" s="17"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="13"/>
       <c r="B20" s="7" t="s">
         <v>16</v>
@@ -2579,15 +3353,15 @@
         <f>IF(Deutsch!F20="","",Deutsch!F20)</f>
         <v/>
       </c>
-      <c r="G20" s="5" t="str">
+      <c r="G20" s="14" t="str">
         <f>IF(Deutsch!G20="","",Deutsch!G20)</f>
         <v/>
       </c>
-      <c r="H20" s="5" t="str">
+      <c r="H20" s="14" t="str">
         <f>IF(Deutsch!H20="","",Deutsch!H20)</f>
         <v/>
       </c>
-      <c r="I20" s="5" t="str">
+      <c r="I20" s="15" t="str">
         <f>IF(Deutsch!I20="","",Deutsch!I20)</f>
         <v/>
       </c>
@@ -2599,11 +3373,11 @@
         <f>IF(Deutsch!K20="","",Deutsch!K20)</f>
         <v/>
       </c>
-      <c r="L20" s="5" t="str">
+      <c r="L20" s="14" t="str">
         <f>IF(Deutsch!L20="","",Deutsch!L20)</f>
         <v/>
       </c>
-      <c r="M20" s="5" t="str">
+      <c r="M20" s="15" t="str">
         <f>IF(Deutsch!M20="","",Deutsch!M20)</f>
         <v/>
       </c>
@@ -2615,12 +3389,13 @@
         <f>IF(Deutsch!O20="","",Deutsch!O20)</f>
         <v/>
       </c>
-      <c r="P20" s="5" t="str">
+      <c r="P20" s="14" t="str">
         <f>IF(Deutsch!P20="","",Deutsch!P20)</f>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" s="17"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="13" t="s">
         <v>41</v>
       </c>
@@ -2643,15 +3418,15 @@
         <f>IF(Deutsch!F21="","",Deutsch!F21)</f>
         <v/>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="14">
         <f>IF(Deutsch!G21="","",Deutsch!G21)</f>
         <v>1</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="14">
         <f>IF(Deutsch!H21="","",Deutsch!H21)</f>
         <v>1</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="15">
         <f>IF(Deutsch!I21="","",Deutsch!I21)</f>
         <v>1</v>
       </c>
@@ -2663,11 +3438,11 @@
         <f>IF(Deutsch!K21="","",Deutsch!K21)</f>
         <v>1</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L21" s="14">
         <f>IF(Deutsch!L21="","",Deutsch!L21)</f>
         <v>1</v>
       </c>
-      <c r="M21" s="5" t="str">
+      <c r="M21" s="15" t="str">
         <f>IF(Deutsch!M21="","",Deutsch!M21)</f>
         <v/>
       </c>
@@ -2679,12 +3454,13 @@
         <f>IF(Deutsch!O21="","",Deutsch!O21)</f>
         <v/>
       </c>
-      <c r="P21" s="5" t="str">
+      <c r="P21" s="14" t="str">
         <f>IF(Deutsch!P21="","",Deutsch!P21)</f>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="17"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="13"/>
       <c r="B22" s="7" t="s">
         <v>16</v>
@@ -2705,15 +3481,15 @@
         <f>IF(Deutsch!F22="","",Deutsch!F22)</f>
         <v/>
       </c>
-      <c r="G22" s="5" t="str">
+      <c r="G22" s="14">
         <f>IF(Deutsch!G22="","",Deutsch!G22)</f>
-        <v/>
-      </c>
-      <c r="H22" s="5" t="str">
+        <v>2</v>
+      </c>
+      <c r="H22" s="14" t="str">
         <f>IF(Deutsch!H22="","",Deutsch!H22)</f>
         <v/>
       </c>
-      <c r="I22" s="5" t="str">
+      <c r="I22" s="15" t="str">
         <f>IF(Deutsch!I22="","",Deutsch!I22)</f>
         <v/>
       </c>
@@ -2725,11 +3501,11 @@
         <f>IF(Deutsch!K22="","",Deutsch!K22)</f>
         <v/>
       </c>
-      <c r="L22" s="5" t="str">
+      <c r="L22" s="14" t="str">
         <f>IF(Deutsch!L22="","",Deutsch!L22)</f>
         <v/>
       </c>
-      <c r="M22" s="5" t="str">
+      <c r="M22" s="15" t="str">
         <f>IF(Deutsch!M22="","",Deutsch!M22)</f>
         <v/>
       </c>
@@ -2741,12 +3517,13 @@
         <f>IF(Deutsch!O22="","",Deutsch!O22)</f>
         <v/>
       </c>
-      <c r="P22" s="5" t="str">
+      <c r="P22" s="14" t="str">
         <f>IF(Deutsch!P22="","",Deutsch!P22)</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22" s="17"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="12" t="s">
         <v>42</v>
       </c>
@@ -2769,15 +3546,15 @@
         <f>IF(Deutsch!F23="","",Deutsch!F23)</f>
         <v/>
       </c>
-      <c r="G23" s="5" t="str">
+      <c r="G23" s="14" t="str">
         <f>IF(Deutsch!G23="","",Deutsch!G23)</f>
         <v/>
       </c>
-      <c r="H23" s="5" t="str">
+      <c r="H23" s="14" t="str">
         <f>IF(Deutsch!H23="","",Deutsch!H23)</f>
         <v/>
       </c>
-      <c r="I23" s="5" t="str">
+      <c r="I23" s="15" t="str">
         <f>IF(Deutsch!I23="","",Deutsch!I23)</f>
         <v/>
       </c>
@@ -2789,11 +3566,11 @@
         <f>IF(Deutsch!K23="","",Deutsch!K23)</f>
         <v/>
       </c>
-      <c r="L23" s="5" t="str">
+      <c r="L23" s="14" t="str">
         <f>IF(Deutsch!L23="","",Deutsch!L23)</f>
         <v/>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="15">
         <f>IF(Deutsch!M23="","",Deutsch!M23)</f>
         <v>1</v>
       </c>
@@ -2805,12 +3582,13 @@
         <f>IF(Deutsch!O23="","",Deutsch!O23)</f>
         <v>1</v>
       </c>
-      <c r="P23" s="5">
+      <c r="P23" s="14">
         <f>IF(Deutsch!P23="","",Deutsch!P23)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="Q23" s="17"/>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="13"/>
       <c r="B24" s="7" t="s">
         <v>16</v>
@@ -2831,15 +3609,15 @@
         <f>IF(Deutsch!F24="","",Deutsch!F24)</f>
         <v/>
       </c>
-      <c r="G24" s="5" t="str">
+      <c r="G24" s="14" t="str">
         <f>IF(Deutsch!G24="","",Deutsch!G24)</f>
         <v/>
       </c>
-      <c r="H24" s="5" t="str">
+      <c r="H24" s="14" t="str">
         <f>IF(Deutsch!H24="","",Deutsch!H24)</f>
         <v/>
       </c>
-      <c r="I24" s="5" t="str">
+      <c r="I24" s="15" t="str">
         <f>IF(Deutsch!I24="","",Deutsch!I24)</f>
         <v/>
       </c>
@@ -2851,11 +3629,11 @@
         <f>IF(Deutsch!K24="","",Deutsch!K24)</f>
         <v/>
       </c>
-      <c r="L24" s="5" t="str">
+      <c r="L24" s="14" t="str">
         <f>IF(Deutsch!L24="","",Deutsch!L24)</f>
         <v/>
       </c>
-      <c r="M24" s="5" t="str">
+      <c r="M24" s="15" t="str">
         <f>IF(Deutsch!M24="","",Deutsch!M24)</f>
         <v/>
       </c>
@@ -2867,12 +3645,13 @@
         <f>IF(Deutsch!O24="","",Deutsch!O24)</f>
         <v/>
       </c>
-      <c r="P24" s="5" t="str">
+      <c r="P24" s="14" t="str">
         <f>IF(Deutsch!P24="","",Deutsch!P24)</f>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24" s="17"/>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="13" t="s">
         <v>43</v>
       </c>
@@ -2895,15 +3674,15 @@
         <f>IF(Deutsch!F25="","",Deutsch!F25)</f>
         <v/>
       </c>
-      <c r="G25" s="5" t="str">
+      <c r="G25" s="14" t="str">
         <f>IF(Deutsch!G25="","",Deutsch!G25)</f>
         <v/>
       </c>
-      <c r="H25" s="5" t="str">
+      <c r="H25" s="14" t="str">
         <f>IF(Deutsch!H25="","",Deutsch!H25)</f>
         <v/>
       </c>
-      <c r="I25" s="5" t="str">
+      <c r="I25" s="15" t="str">
         <f>IF(Deutsch!I25="","",Deutsch!I25)</f>
         <v/>
       </c>
@@ -2915,11 +3694,11 @@
         <f>IF(Deutsch!K25="","",Deutsch!K25)</f>
         <v/>
       </c>
-      <c r="L25" s="5" t="str">
+      <c r="L25" s="14" t="str">
         <f>IF(Deutsch!L25="","",Deutsch!L25)</f>
         <v/>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="15">
         <f>IF(Deutsch!M25="","",Deutsch!M25)</f>
         <v>1</v>
       </c>
@@ -2931,12 +3710,13 @@
         <f>IF(Deutsch!O25="","",Deutsch!O25)</f>
         <v>1</v>
       </c>
-      <c r="P25" s="5">
+      <c r="P25" s="14">
         <f>IF(Deutsch!P25="","",Deutsch!P25)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="17"/>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="13"/>
       <c r="B26" s="7" t="s">
         <v>16</v>
@@ -2957,15 +3737,15 @@
         <f>IF(Deutsch!F26="","",Deutsch!F26)</f>
         <v/>
       </c>
-      <c r="G26" s="5" t="str">
+      <c r="G26" s="14" t="str">
         <f>IF(Deutsch!G26="","",Deutsch!G26)</f>
         <v/>
       </c>
-      <c r="H26" s="5" t="str">
+      <c r="H26" s="14" t="str">
         <f>IF(Deutsch!H26="","",Deutsch!H26)</f>
         <v/>
       </c>
-      <c r="I26" s="5" t="str">
+      <c r="I26" s="15" t="str">
         <f>IF(Deutsch!I26="","",Deutsch!I26)</f>
         <v/>
       </c>
@@ -2977,11 +3757,11 @@
         <f>IF(Deutsch!K26="","",Deutsch!K26)</f>
         <v/>
       </c>
-      <c r="L26" s="5" t="str">
+      <c r="L26" s="14" t="str">
         <f>IF(Deutsch!L26="","",Deutsch!L26)</f>
         <v/>
       </c>
-      <c r="M26" s="5" t="str">
+      <c r="M26" s="15" t="str">
         <f>IF(Deutsch!M26="","",Deutsch!M26)</f>
         <v/>
       </c>
@@ -2993,32 +3773,63 @@
         <f>IF(Deutsch!O26="","",Deutsch!O26)</f>
         <v/>
       </c>
-      <c r="P26" s="5" t="str">
+      <c r="P26" s="14" t="str">
         <f>IF(Deutsch!P26="","",Deutsch!P26)</f>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" s="17"/>
+    </row>
+    <row r="27" spans="1:18" ht="15" customHeight="1">
       <c r="A27" s="11"/>
       <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="H27" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" s="16"/>
+      <c r="L27" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M27" s="16"/>
+      <c r="P27" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q27" s="19"/>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="11"/>
       <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="G28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="11"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:18">
       <c r="A30" s="11"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:18">
       <c r="A31" s="11"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:18">
       <c r="A32" s="11"/>
       <c r="B32" s="2"/>
     </row>
@@ -3031,7 +3842,19 @@
       <c r="B34" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="22">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="O28:R28"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
@@ -3042,26 +3865,70 @@
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <conditionalFormatting sqref="Q21 C2:P26">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="15" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="16" operator="equal">
       <formula>2</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="17" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:P26">
+    <cfRule type="cellIs" dxfId="53" priority="12" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="13" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:P26">
+    <cfRule type="cellIs" dxfId="46" priority="8" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="9" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="10" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:P26 Q21">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:P26">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>3</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Final version of documentation.
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="680" windowWidth="22040" windowHeight="15800"/>
+    <workbookView xWindow="1240" yWindow="1120" windowWidth="22040" windowHeight="15800"/>
   </bookViews>
   <sheets>
     <sheet name="Deutsch" sheetId="1" r:id="rId1"/>
@@ -80,10 +80,6 @@
     <t>Einführung und Besichtigung des  Fahrsimulators</t>
   </si>
   <si>
-    <t>Simulator auf den PC mit Beamer laden 
-und allfällige Fehler beseitigen</t>
-  </si>
-  <si>
     <t>Woche 38</t>
   </si>
   <si>
@@ -148,12 +144,6 @@
     <t>LabVIEW installieren</t>
   </si>
   <si>
-    <t>LabVIEW Schnittstelle initialisieren</t>
-  </si>
-  <si>
-    <t>Film durch Drücken der Pedale steuern (Frame gesteuertes fahren)</t>
-  </si>
-  <si>
     <t>Eigene kleine 3D-Welt kreieren (ev. mit Tunnel)</t>
   </si>
   <si>
@@ -169,7 +159,17 @@
     <t>Einzelne Elemente aus Google 3D Warehouse in unsere 3D-Welt integrieren</t>
   </si>
   <si>
-    <t>3D Framework aufsetzen und Beispiele laufen lassen</t>
+    <t>3D-Framework aufsetzen und Beispiele laufen lassen</t>
+  </si>
+  <si>
+    <t>LabVIEW-Schnittstelle initialisieren</t>
+  </si>
+  <si>
+    <t>Film durch Drücken der Pedale steuern (framegesteuertes fahren)</t>
+  </si>
+  <si>
+    <t>Simulator auf den PC mit Projektor laden 
+und allfällige Fehler beseitigen</t>
   </si>
 </sst>
 </file>
@@ -354,6 +354,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -362,15 +371,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -986,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A28"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1000,7 +1000,7 @@
     <row r="1" spans="1:17" s="1" customFormat="1" ht="57.75" customHeight="1">
       <c r="A1" s="3"/>
       <c r="C1" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>2</v>
@@ -1066,163 +1066,163 @@
       <c r="Q2" s="17"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="22" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="26"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" s="12"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="23" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" s="5">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="12"/>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="26" t="s">
-        <v>40</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="26"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="5">
         <v>2</v>
@@ -1231,52 +1231,52 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -1288,95 +1288,95 @@
         <v>1</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="12"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="26"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="5">
         <v>2</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q8" s="12"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="26" t="s">
-        <v>41</v>
+      <c r="A9" s="23" t="s">
+        <v>46</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
@@ -1388,44 +1388,44 @@
         <v>1</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q9" s="12"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="26"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="5">
         <v>2</v>
@@ -1434,55 +1434,55 @@
         <v>2</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="25" t="s">
-        <v>42</v>
+      <c r="A11" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -1491,41 +1491,41 @@
         <v>1</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="26"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5">
@@ -1538,52 +1538,52 @@
         <v>2</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="25" t="s">
-        <v>48</v>
+      <c r="A13" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" s="10">
         <v>1</v>
@@ -1592,44 +1592,44 @@
         <v>1</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="26"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="10">
         <v>4</v>
@@ -1638,55 +1638,55 @@
         <v>2</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="25" t="s">
-        <v>43</v>
+      <c r="A15" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I15" s="11">
         <v>1</v>
@@ -1701,35 +1701,35 @@
         <v>1</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P15" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="26"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="10">
         <v>4</v>
@@ -1750,46 +1750,46 @@
         <v>2</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="25" t="s">
-        <v>44</v>
+      <c r="A17" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J17" s="5">
         <v>1</v>
@@ -1801,44 +1801,44 @@
         <v>1</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="26"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J18" s="5">
         <v>2</v>
@@ -1853,43 +1853,43 @@
         <v>3</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="25" t="s">
-        <v>47</v>
+      <c r="A19" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J19" s="5">
         <v>1</v>
@@ -1901,50 +1901,50 @@
         <v>1</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P19" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="26"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L20" s="10">
         <v>2</v>
@@ -1956,31 +1956,31 @@
         <v>3</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q20" s="12"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="26" t="s">
-        <v>45</v>
+      <c r="A21" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
@@ -2001,35 +2001,35 @@
         <v>1</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q21" s="12"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="26"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G22" s="10">
         <v>2</v>
@@ -2056,49 +2056,49 @@
         <v>3</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q22" s="12"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="25" t="s">
-        <v>19</v>
+      <c r="A23" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M23" s="11">
         <v>1</v>
@@ -2115,27 +2115,27 @@
       <c r="Q23" s="12"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="26"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I24" s="11">
         <v>4</v>
@@ -2154,49 +2154,49 @@
       </c>
       <c r="N24" s="5"/>
       <c r="O24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q24" s="12"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="26" t="s">
-        <v>46</v>
+      <c r="A25" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M25" s="11">
         <v>1</v>
@@ -2213,42 +2213,42 @@
       <c r="Q25" s="12"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="26"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5">
@@ -2260,69 +2260,75 @@
       <c r="Q26" s="12"/>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1">
-      <c r="A27" s="24"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="2"/>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="24"/>
+      <c r="L27" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" s="24"/>
+      <c r="P27" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q27" s="25"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="21"/>
+      <c r="B28" s="2"/>
+      <c r="G28" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I27" s="21"/>
-      <c r="L27" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="M27" s="21"/>
-      <c r="P27" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q27" s="22"/>
-    </row>
-    <row r="28" spans="1:18">
-      <c r="A28" s="24"/>
-      <c r="B28" s="2"/>
-      <c r="G28" s="23" t="s">
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23" t="s">
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="24"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="24"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="24"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="24"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="24"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="24"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="O28:R28"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
@@ -2339,12 +2345,6 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="O28:R28"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:P26 Q21">
     <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
@@ -2424,7 +2424,7 @@
     <row r="1" spans="1:17" s="1" customFormat="1" ht="57.75" customHeight="1">
       <c r="A1" s="3"/>
       <c r="C1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>2</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -2490,8 +2490,8 @@
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="25" t="s">
-        <v>23</v>
+      <c r="A3" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>15</v>
@@ -2555,7 +2555,7 @@
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="26"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
@@ -2618,8 +2618,8 @@
       <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="26" t="s">
-        <v>24</v>
+      <c r="A5" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>15</v>
@@ -2683,7 +2683,7 @@
       <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="26"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
@@ -2746,8 +2746,8 @@
       <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="26" t="s">
-        <v>25</v>
+      <c r="A7" s="23" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -2811,7 +2811,7 @@
       <c r="Q7" s="12"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="26"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
@@ -2874,8 +2874,8 @@
       <c r="Q8" s="12"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="26" t="s">
-        <v>26</v>
+      <c r="A9" s="23" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
@@ -2939,7 +2939,7 @@
       <c r="Q9" s="12"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="26"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -3002,8 +3002,8 @@
       <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1">
-      <c r="A11" s="25" t="s">
-        <v>27</v>
+      <c r="A11" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>15</v>
@@ -3067,7 +3067,7 @@
       <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="26"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
@@ -3130,8 +3130,8 @@
       <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1">
-      <c r="A13" s="25" t="s">
-        <v>28</v>
+      <c r="A13" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>15</v>
@@ -3195,7 +3195,7 @@
       <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="26"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
@@ -3258,8 +3258,8 @@
       <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1">
-      <c r="A15" s="25" t="s">
-        <v>29</v>
+      <c r="A15" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>15</v>
@@ -3323,7 +3323,7 @@
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="26"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
@@ -3386,8 +3386,8 @@
       <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="25" t="s">
-        <v>30</v>
+      <c r="A17" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>15</v>
@@ -3451,7 +3451,7 @@
       <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="26"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
@@ -3514,8 +3514,8 @@
       <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="25" t="s">
-        <v>31</v>
+      <c r="A19" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>15</v>
@@ -3579,7 +3579,7 @@
       <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="26"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="6" t="s">
         <v>16</v>
       </c>
@@ -3642,8 +3642,8 @@
       <c r="Q20" s="12"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="26" t="s">
-        <v>32</v>
+      <c r="A21" s="23" t="s">
+        <v>31</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>15</v>
@@ -3707,7 +3707,7 @@
       <c r="Q21" s="12"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="26"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
@@ -3770,8 +3770,8 @@
       <c r="Q22" s="12"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="25" t="s">
-        <v>33</v>
+      <c r="A23" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>15</v>
@@ -3835,7 +3835,7 @@
       <c r="Q23" s="12"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="26"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6" t="s">
         <v>16</v>
       </c>
@@ -3898,8 +3898,8 @@
       <c r="Q24" s="12"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="26" t="s">
-        <v>34</v>
+      <c r="A25" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>15</v>
@@ -3963,7 +3963,7 @@
       <c r="Q25" s="12"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="26"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="6" t="s">
         <v>16</v>
       </c>
@@ -4026,69 +4026,82 @@
       <c r="Q26" s="12"/>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1">
-      <c r="A27" s="24"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="2"/>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="24"/>
+      <c r="L27" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" s="24"/>
+      <c r="P27" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q27" s="25"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="21"/>
+      <c r="B28" s="2"/>
+      <c r="G28" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I27" s="21"/>
-      <c r="L27" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="M27" s="21"/>
-      <c r="P27" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q27" s="22"/>
-    </row>
-    <row r="28" spans="1:18">
-      <c r="A28" s="24"/>
-      <c r="B28" s="2"/>
-      <c r="G28" s="23" t="s">
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23" t="s">
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="24"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="24"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="24"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="24"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="24"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="24"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="O28:R28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A33:A34"/>
@@ -4098,19 +4111,6 @@
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="O28:R28"/>
-    <mergeCell ref="A27:A28"/>
   </mergeCells>
   <conditionalFormatting sqref="Q21 C2:P26">
     <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">

</xml_diff>